<commit_message>
checkpoint before switching organization to include global functions module for common functions
</commit_message>
<xml_diff>
--- a/Extracted data.xlsx
+++ b/Extracted data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ualbertaca-my.sharepoint.com/personal/hqiu1_ualberta_ca/Documents/Lab (Taufik)/NeuromodulationNLP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="8_{A3C0C69F-4D60-4F0C-A285-8DF279F49CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FD9F5CC-3F32-4440-A463-750C654BF5E6}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="8_{A3C0C69F-4D60-4F0C-A285-8DF279F49CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8022BDFF-5546-4B16-BC8D-AFDC41182B83}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{AC3F3703-E59A-4C00-A89B-F9AB7B899524}"/>
   </bookViews>
@@ -450,10 +450,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -753,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA43D962-FBAD-4C75-85BD-75903244C543}">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -766,11 +762,13 @@
     <col min="3" max="3" width="11.5" customWidth="1"/>
     <col min="4" max="4" width="11.90625" customWidth="1"/>
     <col min="5" max="5" width="16.04296875" customWidth="1"/>
-    <col min="6" max="7" width="8.7265625" style="1"/>
-    <col min="9" max="16384" width="8.7265625" style="1"/>
+    <col min="6" max="6" width="4.1796875" customWidth="1"/>
+    <col min="7" max="7" width="11.58984375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" style="1"/>
+    <col min="10" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A1" s="3" t="s">
         <v>71</v>
       </c>
@@ -786,11 +784,12 @@
       <c r="E1" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A2" s="1">
         <v>6</v>
       </c>
@@ -806,12 +805,15 @@
       <c r="E2" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A3" s="1">
         <v>14</v>
       </c>
@@ -827,12 +829,15 @@
       <c r="E3" t="s">
         <v>74</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A4" s="1">
         <v>19</v>
       </c>
@@ -848,12 +853,15 @@
       <c r="E4" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A5" s="1">
         <v>22</v>
       </c>
@@ -869,12 +877,15 @@
       <c r="E5" t="s">
         <v>74</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A6" s="1">
         <v>41</v>
       </c>
@@ -890,12 +901,15 @@
       <c r="E6" t="s">
         <v>74</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A7" s="1">
         <v>45</v>
       </c>
@@ -911,12 +925,15 @@
       <c r="E7" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A8" s="1">
         <v>61</v>
       </c>
@@ -932,12 +949,15 @@
       <c r="E8" t="s">
         <v>74</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A9" s="1">
         <v>65</v>
       </c>
@@ -953,12 +973,15 @@
       <c r="E9" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A10" s="1">
         <v>67</v>
       </c>
@@ -974,12 +997,15 @@
       <c r="E10" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A11" s="1">
         <v>68</v>
       </c>
@@ -995,12 +1021,15 @@
       <c r="E11" t="s">
         <v>74</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11">
+        <v>9</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A12" s="1">
         <v>103</v>
       </c>
@@ -1016,12 +1045,15 @@
       <c r="E12" t="s">
         <v>74</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A13" s="1">
         <v>107</v>
       </c>
@@ -1037,12 +1069,15 @@
       <c r="E13" t="s">
         <v>74</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13">
+        <v>11</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A14" s="1">
         <v>110</v>
       </c>
@@ -1058,12 +1093,15 @@
       <c r="E14" t="s">
         <v>74</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14">
+        <v>12</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A15" s="1">
         <v>111</v>
       </c>
@@ -1079,12 +1117,15 @@
       <c r="E15" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15">
+        <v>13</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A16" s="1">
         <v>116</v>
       </c>
@@ -1100,12 +1141,15 @@
       <c r="E16" t="s">
         <v>74</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16">
+        <v>14</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A17" s="1">
         <v>130</v>
       </c>
@@ -1121,12 +1165,15 @@
       <c r="E17" t="s">
         <v>74</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17">
+        <v>15</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A18" s="1">
         <v>147</v>
       </c>
@@ -1142,12 +1189,15 @@
       <c r="E18" t="s">
         <v>74</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18">
+        <v>16</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A19" s="1">
         <v>163</v>
       </c>
@@ -1163,12 +1213,15 @@
       <c r="E19" t="s">
         <v>74</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19">
+        <v>17</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A20" s="1">
         <v>174</v>
       </c>
@@ -1184,12 +1237,15 @@
       <c r="E20" t="s">
         <v>74</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20">
+        <v>18</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A21" s="1">
         <v>175</v>
       </c>
@@ -1205,12 +1261,15 @@
       <c r="E21" t="s">
         <v>74</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21">
+        <v>19</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A22" s="1">
         <v>178</v>
       </c>
@@ -1226,12 +1285,15 @@
       <c r="E22" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22">
+        <v>20</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A23" s="1">
         <v>192</v>
       </c>
@@ -1247,12 +1309,15 @@
       <c r="E23" t="s">
         <v>74</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23">
+        <v>21</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A24" s="1">
         <v>193</v>
       </c>
@@ -1268,12 +1333,15 @@
       <c r="E24" t="s">
         <v>74</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24">
+        <v>22</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A25" s="1">
         <v>211</v>
       </c>
@@ -1289,12 +1357,15 @@
       <c r="E25" t="s">
         <v>74</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25">
+        <v>23</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A26" s="1">
         <v>223</v>
       </c>
@@ -1310,12 +1381,15 @@
       <c r="E26" t="s">
         <v>74</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26">
+        <v>24</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A27" s="1">
         <v>239</v>
       </c>
@@ -1331,12 +1405,15 @@
       <c r="E27" t="s">
         <v>74</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27">
+        <v>25</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A28" s="1">
         <v>242</v>
       </c>
@@ -1352,12 +1429,15 @@
       <c r="E28" t="s">
         <v>74</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28">
+        <v>26</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A29" s="1">
         <v>250</v>
       </c>
@@ -1373,12 +1453,15 @@
       <c r="E29" t="s">
         <v>74</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29">
+        <v>27</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A30" s="1">
         <v>252</v>
       </c>
@@ -1394,12 +1477,15 @@
       <c r="E30" t="s">
         <v>74</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30">
+        <v>28</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A31" s="1">
         <v>269</v>
       </c>
@@ -1415,12 +1501,15 @@
       <c r="E31" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F31">
+        <v>29</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G31" s="2"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A32" s="1">
         <v>291</v>
       </c>
@@ -1436,12 +1525,15 @@
       <c r="E32" t="s">
         <v>74</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F32">
+        <v>30</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G32" s="2"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A33" s="1">
         <v>294</v>
       </c>
@@ -1457,12 +1549,15 @@
       <c r="E33" t="s">
         <v>74</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F33">
+        <v>31</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G33" s="2"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A34" s="1">
         <v>308</v>
       </c>
@@ -1478,12 +1573,15 @@
       <c r="E34" t="s">
         <v>74</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F34">
+        <v>32</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A35" s="1">
         <v>324</v>
       </c>
@@ -1499,12 +1597,15 @@
       <c r="E35" t="s">
         <v>74</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F35">
+        <v>33</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A36" s="1">
         <v>340</v>
       </c>
@@ -1520,12 +1621,15 @@
       <c r="E36" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="F36">
+        <v>34</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G36" s="2"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A37" s="1">
         <v>342</v>
       </c>
@@ -1541,12 +1645,15 @@
       <c r="E37" t="s">
         <v>74</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F37">
+        <v>35</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G37" s="2"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A38" s="1">
         <v>353</v>
       </c>
@@ -1562,12 +1669,15 @@
       <c r="E38" t="s">
         <v>74</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="F38">
+        <v>36</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G38" s="2"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A39" s="1">
         <v>354</v>
       </c>
@@ -1583,12 +1693,15 @@
       <c r="E39" t="s">
         <v>74</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F39">
+        <v>37</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G39" s="2"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H39" s="2"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A40" s="1">
         <v>358</v>
       </c>
@@ -1604,12 +1717,15 @@
       <c r="E40" t="s">
         <v>74</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F40">
+        <v>38</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A41" s="1">
         <v>360</v>
       </c>
@@ -1625,12 +1741,15 @@
       <c r="E41" t="s">
         <v>74</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="F41">
+        <v>39</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G41" s="2"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H41" s="2"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A42" s="1">
         <v>361</v>
       </c>
@@ -1646,12 +1765,15 @@
       <c r="E42" t="s">
         <v>74</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F42">
+        <v>40</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G42" s="2"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H42" s="2"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A43" s="1">
         <v>363</v>
       </c>
@@ -1667,12 +1789,15 @@
       <c r="E43" t="s">
         <v>106</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F43">
+        <v>41</v>
+      </c>
+      <c r="G43" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G43" s="2"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H43" s="2"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A44" s="1">
         <v>366</v>
       </c>
@@ -1688,12 +1813,15 @@
       <c r="E44" t="s">
         <v>74</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="F44">
+        <v>42</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G44" s="2"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H44" s="2"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A45" s="1">
         <v>368</v>
       </c>
@@ -1709,12 +1837,15 @@
       <c r="E45" t="s">
         <v>74</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F45">
+        <v>43</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G45" s="2"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H45" s="2"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A46" s="1">
         <v>370</v>
       </c>
@@ -1730,12 +1861,15 @@
       <c r="E46" t="s">
         <v>74</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="F46">
+        <v>44</v>
+      </c>
+      <c r="G46" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G46" s="2"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H46" s="2"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A47" s="1">
         <v>375</v>
       </c>
@@ -1751,12 +1885,15 @@
       <c r="E47" t="s">
         <v>74</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F47">
+        <v>45</v>
+      </c>
+      <c r="G47" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G47" s="2"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H47" s="2"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A48" s="1">
         <v>377</v>
       </c>
@@ -1772,12 +1909,15 @@
       <c r="E48" t="s">
         <v>74</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="F48">
+        <v>46</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G48" s="2"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H48" s="2"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A49" s="1">
         <v>393</v>
       </c>
@@ -1793,12 +1933,15 @@
       <c r="E49" t="s">
         <v>74</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="F49">
+        <v>47</v>
+      </c>
+      <c r="G49" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G49" s="2"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H49" s="2"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A50" s="1">
         <v>398</v>
       </c>
@@ -1814,12 +1957,15 @@
       <c r="E50" t="s">
         <v>74</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="F50">
+        <v>48</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G50" s="2"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H50" s="2"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A51" s="1">
         <v>419</v>
       </c>
@@ -1835,10 +1981,13 @@
       <c r="E51" t="s">
         <v>74</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="F51">
+        <v>49</v>
+      </c>
+      <c r="G51" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="B1:B51" xr:uid="{AA43D962-FBAD-4C75-85BD-75903244C543}"/>

</xml_diff>